<commit_message>
edit data base on changes in tables
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\courses\university\term 5\az db\project\2\2\Library-Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F992202E-C707-476A-AB65-4CFFD11AF525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0E324B-DFD3-4F00-863E-34EAE5E0F1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="5" xr2:uid="{E4A5B597-1B13-49BD-BC2C-758B64A3650B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{E4A5B597-1B13-49BD-BC2C-758B64A3650B}"/>
   </bookViews>
   <sheets>
     <sheet name="Book" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="238">
   <si>
     <t>bookID</t>
   </si>
@@ -1118,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD73C61-EE14-4FCF-9AAD-FA3086E46927}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E41"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection sqref="A1:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1133,7 +1133,7 @@
     <col min="6" max="6" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1149,8 +1149,11 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1166,8 +1169,11 @@
       <c r="E2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1183,8 +1189,11 @@
       <c r="E3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1200,8 +1209,11 @@
       <c r="E4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1217,8 +1229,11 @@
       <c r="E5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1234,8 +1249,11 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1251,8 +1269,11 @@
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1268,8 +1289,11 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1285,8 +1309,11 @@
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1302,8 +1329,11 @@
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1319,8 +1349,11 @@
       <c r="E11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1336,8 +1369,11 @@
       <c r="E12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1353,8 +1389,11 @@
       <c r="E13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1370,8 +1409,11 @@
       <c r="E14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1387,8 +1429,11 @@
       <c r="E15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1404,8 +1449,11 @@
       <c r="E16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1421,8 +1469,11 @@
       <c r="E17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1438,8 +1489,11 @@
       <c r="E18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1455,8 +1509,11 @@
       <c r="E19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1472,8 +1529,11 @@
       <c r="E20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1489,8 +1549,11 @@
       <c r="E21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1506,8 +1569,11 @@
       <c r="E22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1523,8 +1589,11 @@
       <c r="E23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1540,8 +1609,11 @@
       <c r="E24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1557,8 +1629,11 @@
       <c r="E25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1574,8 +1649,11 @@
       <c r="E26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1591,8 +1669,11 @@
       <c r="E27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1608,8 +1689,11 @@
       <c r="E28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1625,8 +1709,11 @@
       <c r="E29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1642,8 +1729,11 @@
       <c r="E30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1659,8 +1749,11 @@
       <c r="E31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1676,8 +1769,11 @@
       <c r="E32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1693,8 +1789,11 @@
       <c r="E33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1710,8 +1809,11 @@
       <c r="E34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1727,8 +1829,11 @@
       <c r="E35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1744,8 +1849,11 @@
       <c r="E36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1761,8 +1869,11 @@
       <c r="E37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1778,8 +1889,11 @@
       <c r="E38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1795,8 +1909,11 @@
       <c r="E39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1812,8 +1929,11 @@
       <c r="E40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1828,6 +1948,9 @@
       </c>
       <c r="E41">
         <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2344,10 +2467,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3A6BD9-2838-4130-8135-8E8B6DE0070D}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection sqref="A1:C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2356,466 +2479,340 @@
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
         <v>6</v>
       </c>
-      <c r="C15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
         <v>6</v>
       </c>
-      <c r="C17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
         <v>7</v>
       </c>
-      <c r="C19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
-      <c r="C21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
-      <c r="C22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
         <v>4</v>
       </c>
-      <c r="C23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
         <v>5</v>
       </c>
-      <c r="C24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
-      <c r="C25" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
         <v>3</v>
       </c>
-      <c r="C26" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
         <v>4</v>
       </c>
-      <c r="C28" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
-      <c r="C29" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
         <v>6</v>
       </c>
-      <c r="C30" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
-      <c r="C31" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
-      <c r="C32" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
         <v>7</v>
       </c>
-      <c r="C33" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
-      <c r="C34" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
         <v>5</v>
       </c>
-      <c r="C36" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
         <v>5</v>
       </c>
-      <c r="C37" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
-      <c r="C38" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
-      <c r="C39" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
         <v>7</v>
       </c>
-      <c r="C41" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
         <v>8</v>
-      </c>
-      <c r="C42" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2939,7 +2936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBC36CD-2135-4CFD-93D9-706557EA513D}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A56" workbookViewId="0">
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>

</xml_diff>